<commit_message>
Add total score and order; Add a large log file for test.
</commit_message>
<xml_diff>
--- a/data/score.xlsx
+++ b/data/score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWorkSpace\ResearchingProjects\spark-study-maven\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{C4B75050-61FA-4B38-BCD6-EAF094915CAE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{111C9FBD-4D27-42A2-96FE-2C3D899F3CF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10815" xr2:uid="{B5CC1373-B497-4818-9512-4EB96F9569D1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="61">
   <si>
     <t>王晓岚</t>
   </si>
@@ -100,12 +100,120 @@
   </si>
   <si>
     <t>音乐</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 88.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 98.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 85.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 87.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 89.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 73.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 91.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 97.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 72.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 61.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 79.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 68.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 76.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 94.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 100.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 95.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 90.0</t>
+  </si>
+  <si>
+    <t>数学 -&gt; 83.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 92.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 85.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 93.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 98.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 90.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 99.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 83.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 88.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 84.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 64.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 79.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 63.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 89.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 62.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 65.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 74.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 77.0</t>
+  </si>
+  <si>
+    <t>音乐 -&gt; 91.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,8 +282,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{43DCAE26-E30A-4988-9919-E31FB8A17B9C}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -484,15 +620,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1EE5DB-766D-4829-99F2-352E23D7CA4A}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -503,7 +642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,14 +651,17 @@
       </c>
       <c r="C2">
         <f ca="1">ROUND(D2, 0)</f>
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D2">
         <f ca="1">60+RAND()*40</f>
-        <v>86.277580806032091</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68.505694174365075</v>
+      </c>
+      <c r="G2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -528,14 +670,17 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C61" ca="1" si="0">ROUND(D3, 0)</f>
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D61" ca="1" si="1">60+RAND()*40</f>
-        <v>62.456417061923169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.138707035617685</v>
+      </c>
+      <c r="G3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -544,14 +689,17 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>98.050930551005521</v>
+      </c>
+      <c r="G4">
         <v>93</v>
       </c>
-      <c r="D4">
-        <f t="shared" ca="1" si="1"/>
-        <v>93.472919540709569</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -560,14 +708,17 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>90.977171247463218</v>
+      </c>
+      <c r="G5">
         <v>70</v>
       </c>
-      <c r="D5">
-        <f t="shared" ca="1" si="1"/>
-        <v>70.026158532711435</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,14 +727,17 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>70.230375783481861</v>
+      </c>
+      <c r="G6">
         <v>89</v>
       </c>
-      <c r="D6">
-        <f t="shared" ca="1" si="1"/>
-        <v>88.611764378463192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -592,14 +746,17 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>93.028054050284737</v>
+      </c>
+      <c r="G7">
         <v>95</v>
       </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="1"/>
-        <v>95.479820830844361</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -608,14 +765,17 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>66.397625279399008</v>
+      </c>
+      <c r="G8">
         <v>94</v>
       </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="1"/>
-        <v>93.829690595040887</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -624,14 +784,17 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>60.840727493370544</v>
+      </c>
+      <c r="G9">
         <v>79</v>
       </c>
-      <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>79.109609441248978</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -640,14 +803,17 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>79.252528625850317</v>
+      </c>
+      <c r="G10">
         <v>90</v>
       </c>
-      <c r="D10">
-        <f t="shared" ca="1" si="1"/>
-        <v>90.100459542244096</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -656,14 +822,17 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>86.970740508864964</v>
+      </c>
+      <c r="G11">
         <v>62</v>
       </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="1"/>
-        <v>61.565472063302742</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -672,14 +841,17 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>96.158654677618671</v>
+      </c>
+      <c r="G12">
         <v>82</v>
       </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="1"/>
-        <v>82.039328103855979</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -688,14 +860,17 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="1"/>
+        <v>63.206732442595246</v>
+      </c>
+      <c r="G13">
         <v>92</v>
       </c>
-      <c r="D13">
-        <f t="shared" ca="1" si="1"/>
-        <v>91.586816203243757</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -704,14 +879,17 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="1"/>
+        <v>88.207837439556016</v>
+      </c>
+      <c r="G14">
         <v>75</v>
       </c>
-      <c r="D14">
-        <f t="shared" ca="1" si="1"/>
-        <v>75.346636891516184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -720,14 +898,17 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="1"/>
+        <v>98.522209589685858</v>
+      </c>
+      <c r="G15">
         <v>87</v>
       </c>
-      <c r="D15">
-        <f t="shared" ca="1" si="1"/>
-        <v>87.033957649330176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -736,14 +917,17 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="1"/>
+        <v>61.672567267853822</v>
+      </c>
+      <c r="G16">
         <v>86</v>
       </c>
-      <c r="D16">
-        <f t="shared" ca="1" si="1"/>
-        <v>86.074588087255108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -752,14 +936,17 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>71.765426238311676</v>
+      </c>
+      <c r="G17">
         <v>96</v>
       </c>
-      <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>96.015414319430491</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -768,14 +955,17 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="1"/>
+        <v>68.864043005216644</v>
+      </c>
+      <c r="G18">
         <v>73</v>
       </c>
-      <c r="D18">
-        <f t="shared" ca="1" si="1"/>
-        <v>72.582562988036187</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -784,14 +974,17 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="1"/>
+        <v>88.37865216512121</v>
+      </c>
+      <c r="G19">
         <v>65</v>
       </c>
-      <c r="D19">
-        <f t="shared" ca="1" si="1"/>
-        <v>64.549802821697469</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -800,14 +993,17 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="1"/>
+        <v>80.433144086274126</v>
+      </c>
+      <c r="G20">
         <v>85</v>
       </c>
-      <c r="D20">
-        <f t="shared" ca="1" si="1"/>
-        <v>85.26301809716432</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -816,14 +1012,17 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="1"/>
+        <v>81.84028732796466</v>
+      </c>
+      <c r="G21">
         <v>67</v>
       </c>
-      <c r="D21">
-        <f t="shared" ca="1" si="1"/>
-        <v>66.686914935785055</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -832,14 +1031,17 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>87.752379694393369</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95.385601859704508</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,14 +1050,17 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>98.337668496805804</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.212770337732366</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -864,14 +1069,17 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>85.198474571119647</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.839719923327351</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -880,14 +1088,17 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>86.816807001135928</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.181695930797133</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>4</v>
       </c>
@@ -896,14 +1107,17 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>89.416382200601788</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98.790043274669415</v>
+      </c>
+      <c r="G26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -912,14 +1126,17 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>72.881960764581393</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88.089362651777208</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -928,14 +1145,17 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>90.81277035840084</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.194959429734254</v>
+      </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -944,14 +1164,17 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>96.519446292628771</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70.280964467922175</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -960,14 +1183,17 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>72.252451820299115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70.300948886109694</v>
+      </c>
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -976,14 +1202,17 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>61.007894758877427</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.523831401906762</v>
+      </c>
+      <c r="G31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
@@ -992,14 +1221,17 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
-        <v>78.573431971838275</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.774738798337097</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -1008,14 +1240,17 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
-        <v>67.632667752184972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.151592450332387</v>
+      </c>
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1024,14 +1259,17 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>75.779135624498778</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.81336474142725</v>
+      </c>
+      <c r="G34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1040,14 +1278,17 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>94.301675957837801</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61.103554585151187</v>
+      </c>
+      <c r="G35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1056,14 +1297,17 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>99.749498710008226</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.404675526061723</v>
+      </c>
+      <c r="G36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>15</v>
       </c>
@@ -1072,14 +1316,17 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="1"/>
-        <v>95.077557786193125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93.884372094140218</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -1088,14 +1335,17 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>60.693400532531562</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.039349633844523</v>
+      </c>
+      <c r="G38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
@@ -1104,14 +1354,17 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>90.452261038800202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.768100563435013</v>
+      </c>
+      <c r="G39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -1120,14 +1373,17 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="1"/>
-        <v>83.233841598288251</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79.165366414525806</v>
+      </c>
+      <c r="G40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -1136,14 +1392,17 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>90.549401722320894</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.08111262761193</v>
+      </c>
+      <c r="G41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>0</v>
       </c>
@@ -1152,14 +1411,17 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
-        <v>92.116060897469367</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.511693071562775</v>
+      </c>
+      <c r="G42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
@@ -1168,14 +1430,17 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
-        <v>85.117639077168121</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73.944364672818523</v>
+      </c>
+      <c r="G43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -1184,14 +1449,17 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
-        <v>93.26280620487708</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99.543888526786077</v>
+      </c>
+      <c r="G44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
@@ -1200,14 +1468,17 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
-        <v>98.291359402020746</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.792591915162234</v>
+      </c>
+      <c r="G45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>4</v>
       </c>
@@ -1216,14 +1487,17 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>89.599304711675217</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85.905569739413735</v>
+      </c>
+      <c r="G46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
@@ -1232,14 +1506,17 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>98.813978419470729</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78.131522112681154</v>
+      </c>
+      <c r="G47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
@@ -1248,14 +1525,17 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
-        <v>83.151991327945325</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.060481817398937</v>
+      </c>
+      <c r="G48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -1264,14 +1544,17 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="1"/>
-        <v>88.062859540118524</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82.568688348208994</v>
+      </c>
+      <c r="G49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>8</v>
       </c>
@@ -1280,14 +1563,17 @@
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
-        <v>83.611758910902751</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.538993560618408</v>
+      </c>
+      <c r="G50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>9</v>
       </c>
@@ -1296,14 +1582,17 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>63.978417699963572</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.520793114628646</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>10</v>
       </c>
@@ -1312,14 +1601,17 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="1"/>
-        <v>79.275246444207426</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61.725904426959815</v>
+      </c>
+      <c r="G52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>11</v>
       </c>
@@ -1328,14 +1620,17 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="1"/>
-        <v>83.48796600205165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89.795046734205982</v>
+      </c>
+      <c r="G53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>12</v>
       </c>
@@ -1344,14 +1639,17 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="1"/>
-        <v>62.562567940245543</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65.757408571243644</v>
+      </c>
+      <c r="G54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>13</v>
       </c>
@@ -1360,14 +1658,17 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="1"/>
-        <v>88.978806644884472</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73.341965270685606</v>
+      </c>
+      <c r="G55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>14</v>
       </c>
@@ -1376,14 +1677,17 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="1"/>
-        <v>62.304942463776001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92.615251892922799</v>
+      </c>
+      <c r="G56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
@@ -1392,14 +1696,17 @@
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="1"/>
-        <v>64.817520536741114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.674191244873327</v>
+      </c>
+      <c r="G57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>16</v>
       </c>
@@ -1408,14 +1715,17 @@
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="1"/>
-        <v>74.19146265117152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72.659591732882703</v>
+      </c>
+      <c r="G58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>17</v>
       </c>
@@ -1424,14 +1734,17 @@
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="1"/>
-        <v>77.427577796914122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71.030860319972845</v>
+      </c>
+      <c r="G59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>18</v>
       </c>
@@ -1440,14 +1753,17 @@
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="1"/>
-        <v>63.929735209780738</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68.643849936111323</v>
+      </c>
+      <c r="G60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>18</v>
       </c>
@@ -1456,11 +1772,14 @@
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="1"/>
-        <v>91.056909592952408</v>
+        <v>90.014138137222233</v>
+      </c>
+      <c r="G61" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>